<commit_message>
switch generic parser to using samples instead of individuals, #674
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-measuring.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-measuring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>PIT</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Sex</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -866,18 +869,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
     <col min="15" max="15" width="16.28515625" customWidth="1"/>
     <col min="16" max="16" width="22.140625" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
@@ -885,46 +886,46 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>11</v>
@@ -937,32 +938,32 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="5"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
-      <c r="J2" s="6"/>
+      <c r="F2" s="3"/>
       <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="5"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
-      <c r="J3" s="6"/>
+      <c r="F3" s="3"/>
       <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="3"/>
-      <c r="J4" s="6"/>
+      <c r="F4" s="3"/>
       <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="3"/>
-      <c r="J5" s="6"/>
+      <c r="F5" s="3"/>
       <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>